<commit_message>
Implemented more stuff in BlockAttributesList. Improved GenerationIO.
</commit_message>
<xml_diff>
--- a/TiaAddin-Spin-ExcelReader/z.Excel Configurations/ConfigAllarmiUtenze_Motori.xlsx
+++ b/TiaAddin-Spin-ExcelReader/z.Excel Configurations/ConfigAllarmiUtenze_Motori.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PARONETTO G\Documents\GitHub\TiaAddIn-Spin\TiaAddin-Spin-ExcelReader\z.Excel Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603DF58F-5199-402A-8183-3D9FD35E2F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B388594-27F7-4D57-A0A8-E9BFF2A08830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21960" windowHeight="13176" xr2:uid="{22A793F4-95FD-4AFA-8F43-DC77A5638B57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27750" windowHeight="16440" xr2:uid="{22A793F4-95FD-4AFA-8F43-DC77A5638B57}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -168,12 +168,6 @@
     <t>Nome segmento divisione per utenza</t>
   </si>
   <si>
-    <t>Indirizzo Utenza</t>
-  </si>
-  <si>
-    <t>Prefisso indirizzo utenza</t>
-  </si>
-  <si>
     <t>AlmTimers.Alm[{alarm_num}]</t>
   </si>
   <si>
@@ -195,9 +189,6 @@
     <t>T#3s</t>
   </si>
   <si>
-    <t>Valvola ambidestra con flusso canalizzatore</t>
-  </si>
-  <si>
     <t>TOF</t>
   </si>
   <si>
@@ -226,13 +217,22 @@
   </si>
   <si>
     <t>Imposta \ sul campo indirizzo bobina, set e/o timer per non far generare i corrispettivi. Se il campo è vuoto, verrà usato il valore di default nella config. a sinistra.</t>
+  </si>
+  <si>
+    <t>Valvola ambidestra con flusso canalizzatore 1.21GW</t>
+  </si>
+  <si>
+    <t>Indirizzo Allarme</t>
+  </si>
+  <si>
+    <t>Prefisso indirizzo allarme</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +275,12 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -325,15 +331,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -651,81 +657,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667AB657-9EF0-4E7D-B211-0DE4E07AFF8D}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="2" width="34.21875" customWidth="1"/>
-    <col min="3" max="3" width="71.88671875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="1.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
+    <col min="3" max="3" width="71.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="1.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="15" style="2" customWidth="1"/>
-    <col min="6" max="6" width="45.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="1.44140625" style="2" customWidth="1"/>
-    <col min="8" max="11" width="20.77734375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="5.77734375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="8.77734375" style="7" customWidth="1"/>
-    <col min="14" max="14" width="45.77734375" style="7" customWidth="1"/>
-    <col min="15" max="15" width="5.77734375" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="50.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="1.42578125" style="2" customWidth="1"/>
+    <col min="8" max="11" width="20.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" style="7" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" style="7" customWidth="1"/>
+    <col min="14" max="14" width="45.7109375" style="7" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+    <row r="1" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
       <c r="M1" s="8"/>
     </row>
-    <row r="2" spans="1:15" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="10"/>
+      <c r="E2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="H2" s="9" t="s">
+      <c r="F2" s="10"/>
+      <c r="H2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-    </row>
-    <row r="3" spans="1:15" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+    </row>
+    <row r="3" spans="1:15" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-    </row>
-    <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="H3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+    </row>
+    <row r="4" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
@@ -733,10 +739,10 @@
         <v>2</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>36</v>
@@ -751,7 +757,7 @@
         <v>34</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>0</v>
@@ -760,7 +766,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
@@ -771,13 +777,13 @@
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>35</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>26</v>
@@ -786,7 +792,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
@@ -797,7 +803,7 @@
         <v>38</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>27</v>
@@ -806,12 +812,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H7" s="2" t="s">
         <v>39</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>28</v>
@@ -820,7 +826,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
@@ -831,7 +837,7 @@
         <v>40</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>29</v>
@@ -840,7 +846,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
@@ -851,7 +857,7 @@
         <v>41</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>30</v>
@@ -860,21 +866,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>42</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>31</v>
@@ -883,18 +889,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>43</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>32</v>
@@ -903,12 +909,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H12" s="2" t="s">
         <v>44</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>33</v>
@@ -917,7 +923,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>19</v>
       </c>
@@ -925,7 +931,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>13</v>
       </c>
@@ -933,31 +939,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>25</v>
       </c>
@@ -965,39 +971,39 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1008,6 +1014,7 @@
     <mergeCell ref="B1:K1"/>
     <mergeCell ref="H2:O2"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{F5E4D3FC-4D67-4AB1-A3E0-2BD5870384F2}">
       <formula1>"UnoPerSegmento,GruppoPerSegmento"</formula1>

</xml_diff>

<commit_message>
Added more nodes to BlockAttributeList.
Also improved and refractored both GenerationUserAlarms and GenerationIO.
</commit_message>
<xml_diff>
--- a/TiaAddin-Spin-ExcelReader/z.Excel Configurations/ConfigAllarmiUtenze_Motori.xlsx
+++ b/TiaAddin-Spin-ExcelReader/z.Excel Configurations/ConfigAllarmiUtenze_Motori.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PARONETTO G\Documents\GitHub\TiaAddIn-Spin\TiaAddin-Spin-ExcelReader\z.Excel Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B388594-27F7-4D57-A0A8-E9BFF2A08830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEF94F4-E455-4222-AEFB-AA3711A8C5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27750" windowHeight="16440" xr2:uid="{22A793F4-95FD-4AFA-8F43-DC77A5638B57}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13755" windowHeight="16200" xr2:uid="{22A793F4-95FD-4AFA-8F43-DC77A5638B57}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="71">
   <si>
     <t>Descrizione allarme</t>
   </si>
@@ -48,15 +48,9 @@
     <t>CB01</t>
   </si>
   <si>
-    <t>Formato num. Allarme</t>
-  </si>
-  <si>
     <t>000.###</t>
   </si>
   <si>
-    <t>Num. allarme di partenza</t>
-  </si>
-  <si>
     <t>Usa</t>
   </si>
   <si>
@@ -66,9 +60,6 @@
     <t>false</t>
   </si>
   <si>
-    <t>Salta num. ogni fine gruppo</t>
-  </si>
-  <si>
     <t>Tipo raggruppamento</t>
   </si>
   <si>
@@ -78,33 +69,15 @@
     <t>TYPE1</t>
   </si>
   <si>
-    <t>Dati Blocco FC</t>
-  </si>
-  <si>
     <t>Numero</t>
   </si>
   <si>
-    <t>Num. anti slittamento gruppo</t>
-  </si>
-  <si>
     <t>Indirizzo Timer</t>
   </si>
   <si>
     <t>TON</t>
   </si>
   <si>
-    <t>Default indirizzo bobina</t>
-  </si>
-  <si>
-    <t>Default indirizzo set</t>
-  </si>
-  <si>
-    <t>Default indirizzo timer</t>
-  </si>
-  <si>
-    <t>Default tipo timer</t>
-  </si>
-  <si>
     <t>Timeout marcia avanti motore</t>
   </si>
   <si>
@@ -162,12 +135,6 @@
     <t>Alm.Overtemperature</t>
   </si>
   <si>
-    <t>Nome segmento divisione per allarme</t>
-  </si>
-  <si>
-    <t>Nome segmento divisione per utenza</t>
-  </si>
-  <si>
     <t>AlmTimers.Alm[{alarm_num}]</t>
   </si>
   <si>
@@ -177,9 +144,6 @@
     <t>Descrizione</t>
   </si>
   <si>
-    <t>Default tempo timer</t>
-  </si>
-  <si>
     <t>T#0s</t>
   </si>
   <si>
@@ -225,14 +189,62 @@
     <t>Indirizzo Allarme</t>
   </si>
   <si>
-    <t>Prefisso indirizzo allarme</t>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>Numero allarme</t>
+  </si>
+  <si>
+    <t>Valori default campi</t>
+  </si>
+  <si>
+    <t>Indirizzo bobina</t>
+  </si>
+  <si>
+    <t>Indirizzo set</t>
+  </si>
+  <si>
+    <t>Indirizzo timer</t>
+  </si>
+  <si>
+    <t>Tipo timer</t>
+  </si>
+  <si>
+    <t>Prefissi campi</t>
+  </si>
+  <si>
+    <t>Formato</t>
+  </si>
+  <si>
+    <t>Num. Partenza</t>
+  </si>
+  <si>
+    <t>Salta ogni fine gruppo</t>
+  </si>
+  <si>
+    <t>Anti slittamento gruppo</t>
+  </si>
+  <si>
+    <t>Nome segmento</t>
+  </si>
+  <si>
+    <t>Divisione per allarme</t>
+  </si>
+  <si>
+    <t>Divisione per utenza</t>
+  </si>
+  <si>
+    <t>Indirizzo allarme</t>
+  </si>
+  <si>
+    <t>Valore timer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +297,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -294,7 +314,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -302,20 +322,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -341,6 +419,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -655,359 +763,407 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667AB657-9EF0-4E7D-B211-0DE4E07AFF8D}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1"/>
-    <col min="3" max="3" width="71.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="75" style="2" customWidth="1"/>
     <col min="4" max="4" width="1.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="15" style="2" customWidth="1"/>
     <col min="6" max="6" width="50.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="1.42578125" style="2" customWidth="1"/>
     <col min="8" max="11" width="20.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" style="7" customWidth="1"/>
-    <col min="14" max="14" width="45.7109375" style="7" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" style="6" customWidth="1"/>
+    <col min="14" max="14" width="45.7109375" style="6" customWidth="1"/>
     <col min="15" max="15" width="5.7109375" style="2" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="M1" s="8"/>
+      <c r="B1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:15" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="E2" s="10" t="s">
+      <c r="C2" s="9"/>
+      <c r="E2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="H2" s="10" t="s">
+      <c r="F2" s="9"/>
+      <c r="H2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-    </row>
-    <row r="3" spans="1:15" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" spans="1:15" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
     </row>
     <row r="4" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="B4" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="N4" s="4" t="s">
+      <c r="F4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="O4" s="4" t="s">
-        <v>10</v>
+      <c r="O4" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="14">
+        <v>200</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3">
-        <v>200</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>12</v>
+      <c r="O6" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="H11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="20">
+        <v>200</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="16"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="3">
-        <v>200</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="2" t="s">
+    </row>
+    <row r="23" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B24" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="16"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="12"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="12"/>
+    </row>
+    <row r="28" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+      <c r="C28" s="17"/>
+    </row>
+    <row r="29" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B30" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C30" s="16"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>61</v>
+    <row r="32" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="H3:O3"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="B2:C2"/>
@@ -1016,21 +1172,21 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{F5E4D3FC-4D67-4AB1-A3E0-2BD5870384F2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{F5E4D3FC-4D67-4AB1-A3E0-2BD5870384F2}">
       <formula1>"UnoPerSegmento,GruppoPerSegmento"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8 C6 C13" xr:uid="{F717952B-D4F9-4570-84C1-F92597681F3D}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12 C6 C14" xr:uid="{F717952B-D4F9-4570-84C1-F92597681F3D}">
       <formula1>0</formula1>
       <formula2>99999</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{28CE5F0A-4030-43FD-81FB-F3DA458AE77A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{28CE5F0A-4030-43FD-81FB-F3DA458AE77A}">
       <formula1>"PerUtenza,PerTipoAllarme"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{7DFC26E2-A127-47D5-9AFB-DCB3CF89BE1E}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{7DFC26E2-A127-47D5-9AFB-DCB3CF89BE1E}">
       <formula1>0</formula1>
       <formula2>9999</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19 L5:L1048576" xr:uid="{30675AF6-6451-470D-BF1D-59341B028670}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21 L5:L1048576" xr:uid="{30675AF6-6451-470D-BF1D-59341B028670}">
       <formula1>"TON,TOF"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O1048576" xr:uid="{ABA14625-FEA0-4BF2-8F91-7CEA04EDBD43}">

</xml_diff>

<commit_message>
Fix a bug inside User alarm generation.
</commit_message>
<xml_diff>
--- a/TiaAddin-Spin-ExcelReader/z.Excel Configurations/ConfigAllarmiUtenze_Motori.xlsx
+++ b/TiaAddin-Spin-ExcelReader/z.Excel Configurations/ConfigAllarmiUtenze_Motori.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PARONETTO G\Documents\GitHub\TiaAddIn-Spin\TiaAddin-Spin-ExcelReader\z.Excel Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEF94F4-E455-4222-AEFB-AA3711A8C5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BDEBBB-646B-4AD6-8A56-5B08F6F1DF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13755" windowHeight="16200" xr2:uid="{22A793F4-95FD-4AFA-8F43-DC77A5638B57}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="20640" windowHeight="11835" xr2:uid="{22A793F4-95FD-4AFA-8F43-DC77A5638B57}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -228,16 +228,16 @@
     <t>Nome segmento</t>
   </si>
   <si>
-    <t>Divisione per allarme</t>
-  </si>
-  <si>
-    <t>Divisione per utenza</t>
-  </si>
-  <si>
     <t>Indirizzo allarme</t>
   </si>
   <si>
     <t>Valore timer</t>
+  </si>
+  <si>
+    <t>Divisione uno alla volta</t>
+  </si>
+  <si>
+    <t>Divisione per gruppo</t>
   </si>
 </sst>
 </file>
@@ -388,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -409,16 +409,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -428,27 +418,29 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -765,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667AB657-9EF0-4E7D-B211-0DE4E07AFF8D}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,63 +779,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
       <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:15" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="17"/>
+      <c r="E2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="H2" s="9" t="s">
+      <c r="F2" s="17"/>
+      <c r="H2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
     </row>
     <row r="3" spans="1:15" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
     </row>
     <row r="4" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="15"/>
       <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
@@ -876,10 +868,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -902,10 +894,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="11">
         <v>200</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -993,10 +985,10 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="19"/>
+      <c r="C11" s="15"/>
       <c r="H11" s="2" t="s">
         <v>34</v>
       </c>
@@ -1011,10 +1003,10 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="13">
         <v>200</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -1031,144 +1023,144 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="13">
         <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="16"/>
+      <c r="C17" s="15"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" s="17" t="s">
+      <c r="B22" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="16"/>
+      <c r="C24" s="15"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="12" t="s">
+      <c r="B25" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="12"/>
+      <c r="C26" s="9"/>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="12"/>
+      <c r="C27" s="9"/>
     </row>
     <row r="28" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="17"/>
+      <c r="C28" s="12"/>
     </row>
     <row r="29" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="16"/>
+      <c r="C30" s="15"/>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="12" t="s">
+      <c r="B31" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="17" t="s">
+      <c r="B32" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="H3:O3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="H2:O2"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="H3:O3"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="H2:O2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="6">

</xml_diff>